<commit_message>
primer commit desde JO
</commit_message>
<xml_diff>
--- a/Status.xlsx
+++ b/Status.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,26 +448,74 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>#17 EMBROIDERED JOURNEY ANKLE DRESS - OSMAN</t>
+          <t>#51 FANCY SEA MAXI DRESS - ANDRE</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>#17 EMBROIDERED JOURNEY ANKLE DRESS - OSMAN</t>
+          <t>#88 WESTERN WAVE MIDI SKIRT</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>#26 THE CLASSIC ONE PEACE- CINTURON</t>
+          <t>#138 Y #140  SLIP SKIRT</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>#26 THE CLASSIC ONE PEACE- CINTURON</t>
-        </is>
-      </c>
+          <t>#121 COLLAR DXF</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>#88 WESTERN WAVE MIDI SKIRT</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>#24 COLLAR DXF</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>#100 BOAT LINES TOP-LUZKA</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>#79 COLLAR -NECKLACE DXF</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>#121 COLLAR DXF</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>#24 COLLAR DXF</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>#79 COLLAR -NECKLACE DXF</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>